<commit_message>
new weather data, historic modeling of bordeaux weather and quality
</commit_message>
<xml_diff>
--- a/data/lafitePriceQuality.xlsx
+++ b/data/lafitePriceQuality.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\polin\Dropbox\EE 608 spring 2023\project\Wine-Quality-Modeling\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92390347-B9FD-47C4-893E-7317B529BBF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3932762D-5DD6-4149-92B2-16C090DD8630}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="41955" yWindow="1695" windowWidth="23040" windowHeight="12210" xr2:uid="{CD092E8C-AB39-452C-9685-A8CB2E82F981}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{CD092E8C-AB39-452C-9685-A8CB2E82F981}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="32">
   <si>
     <t>CHATEAU LAFITE ROTHSCHILD</t>
   </si>
@@ -129,6 +129,9 @@
   </si>
   <si>
     <t>quality</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -175,11 +178,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -495,15 +497,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBA3B5D7-1FCE-4B78-9A47-EBE15F83530A}">
-  <dimension ref="A1:E185"/>
+  <dimension ref="A1:M185"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>27</v>
       </c>
@@ -517,7 +519,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -530,14 +532,13 @@
       <c r="D2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="3"/>
-    </row>
-    <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -551,12 +552,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -570,12 +571,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>0</v>
       </c>
@@ -589,12 +590,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -608,12 +609,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>0</v>
       </c>
@@ -627,12 +628,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>0</v>
       </c>
@@ -646,12 +647,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>0</v>
       </c>
@@ -665,12 +666,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>0</v>
       </c>
@@ -683,13 +684,16 @@
       <c r="D18" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M18" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>0</v>
       </c>
@@ -703,12 +707,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>0</v>
       </c>
@@ -722,12 +726,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>0</v>
       </c>
@@ -741,12 +745,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>0</v>
       </c>
@@ -760,12 +764,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>0</v>
       </c>
@@ -779,12 +783,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>0</v>
       </c>
@@ -798,12 +802,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>0</v>
       </c>

</xml_diff>